<commit_message>
Tabela de Busca implementada
</commit_message>
<xml_diff>
--- a/Sprint 5/Sprint_5 Burndown-Backlog.xlsx
+++ b/Sprint 5/Sprint_5 Burndown-Backlog.xlsx
@@ -209,7 +209,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="[$R$ -416]#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -304,6 +304,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
@@ -489,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -549,25 +555,49 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="9" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -606,11 +636,11 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -627,40 +657,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2830,11 +2837,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="205260632"/>
-        <c:axId val="205261024"/>
+        <c:axId val="184086016"/>
+        <c:axId val="184409696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="205260632"/>
+        <c:axId val="184086016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2915,7 +2922,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205261024"/>
+        <c:crossAx val="184409696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2923,7 +2930,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="205261024"/>
+        <c:axId val="184409696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3005,7 +3012,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205260632"/>
+        <c:crossAx val="184086016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3339,11 +3346,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="205262200"/>
-        <c:axId val="205262592"/>
+        <c:axId val="184566664"/>
+        <c:axId val="184649488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="205262200"/>
+        <c:axId val="184566664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3416,7 +3423,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205262592"/>
+        <c:crossAx val="184649488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3424,7 +3431,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="205262592"/>
+        <c:axId val="184649488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3506,7 +3513,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205262200"/>
+        <c:crossAx val="184566664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3840,11 +3847,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208327088"/>
-        <c:axId val="208327480"/>
+        <c:axId val="184309656"/>
+        <c:axId val="185364024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208327088"/>
+        <c:axId val="184309656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3917,7 +3924,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208327480"/>
+        <c:crossAx val="185364024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3925,7 +3932,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208327480"/>
+        <c:axId val="185364024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4007,7 +4014,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208327088"/>
+        <c:crossAx val="184309656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4341,11 +4348,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="208328656"/>
-        <c:axId val="208329048"/>
+        <c:axId val="185275152"/>
+        <c:axId val="186067368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208328656"/>
+        <c:axId val="185275152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4418,7 +4425,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208329048"/>
+        <c:crossAx val="186067368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4426,7 +4433,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208329048"/>
+        <c:axId val="186067368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4508,7 +4515,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208328656"/>
+        <c:crossAx val="185275152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4990,7 +4997,7 @@
   <dimension ref="A1:AB1048572"/>
   <sheetViews>
     <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5007,16 +5014,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5041,27 +5048,27 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="33">
         <v>8</v>
       </c>
       <c r="J2" s="3"/>
@@ -5085,9 +5092,9 @@
       <c r="AB2" s="4"/>
     </row>
     <row r="3" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -5100,8 +5107,8 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -5123,22 +5130,22 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="29">
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="37">
         <f>SUM(F5:F11)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="56"/>
-      <c r="I4" s="52"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -5160,18 +5167,18 @@
       <c r="AB4" s="4"/>
     </row>
     <row r="5" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="56" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="27"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="20"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="57"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="28"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -5192,16 +5199,16 @@
       <c r="AB5" s="4"/>
     </row>
     <row r="6" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="48"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="57" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
-      <c r="E6" s="49"/>
+      <c r="E6" s="35"/>
       <c r="F6" s="20"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="57"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="28"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -5222,16 +5229,16 @@
       <c r="AB6" s="4"/>
     </row>
     <row r="7" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="48"/>
-      <c r="B7" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="58" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="28"/>
+      <c r="E7" s="36"/>
       <c r="F7" s="20"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="57"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="28"/>
       <c r="I7" s="6"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -5253,16 +5260,16 @@
       <c r="AB7" s="4"/>
     </row>
     <row r="8" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
-      <c r="B8" s="51" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="59" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
-      <c r="E8" s="50"/>
+      <c r="E8" s="22"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="57"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="6"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -5284,16 +5291,16 @@
       <c r="AB8" s="4"/>
     </row>
     <row r="9" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="26"/>
-      <c r="B9" s="51" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="59" t="s">
         <v>53</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="50"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="20"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="57"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="28"/>
       <c r="I9" s="6"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -5315,18 +5322,18 @@
       <c r="AB9" s="4"/>
     </row>
     <row r="10" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="56" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
-      <c r="E10" s="27"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="20"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="57"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="28"/>
       <c r="I10" s="6"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -5348,16 +5355,16 @@
       <c r="AB10" s="4"/>
     </row>
     <row r="11" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="32"/>
+      <c r="B11" s="56" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
-      <c r="E11" s="28"/>
+      <c r="E11" s="36"/>
       <c r="F11" s="20"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="57"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="28"/>
       <c r="I11" s="6"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -5637,12 +5644,6 @@
     <row r="1048572" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G4:G11"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -5650,6 +5651,12 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:H3"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G4:G11"/>
   </mergeCells>
   <conditionalFormatting sqref="I1:I4">
     <cfRule type="expression" dxfId="127" priority="2">
@@ -5694,20 +5701,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="33"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -5766,40 +5773,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34">
+      <c r="A3" s="42">
         <v>8</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="J3" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="43" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -5811,18 +5818,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -5971,18 +5978,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -6740,20 +6747,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="33"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -6812,40 +6819,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34">
+      <c r="A3" s="42">
         <v>8</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="43" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -6857,18 +6864,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -7017,18 +7024,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -7094,10 +7101,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="43"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="13">
         <v>0</v>
       </c>
@@ -7131,18 +7138,18 @@
         <v>0.72499999999999998</v>
       </c>
       <c r="M10" s="7"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="46"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="13">
         <v>0</v>
       </c>
@@ -7176,18 +7183,18 @@
         <v>0</v>
       </c>
       <c r="M11" s="7"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="47"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="47"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="13">
         <v>0</v>
       </c>
@@ -7221,18 +7228,18 @@
         <v>0</v>
       </c>
       <c r="M12" s="7"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="41"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="13">
         <v>0</v>
       </c>
@@ -7266,18 +7273,18 @@
         <v>0.74375000000000002</v>
       </c>
       <c r="M13" s="7"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="41"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="13">
         <v>0</v>
       </c>
@@ -7316,16 +7323,6 @@
     <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="N11:O11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A3:A4"/>
@@ -7340,6 +7337,16 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="N13:O13"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:L96">
     <cfRule type="expression" dxfId="26" priority="2">
@@ -7401,20 +7408,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="33"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -7473,40 +7480,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34">
+      <c r="A3" s="42">
         <v>8</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="43" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -7518,18 +7525,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -7678,18 +7685,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -7755,39 +7762,39 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="23">
-        <v>0</v>
-      </c>
-      <c r="D10" s="23">
-        <v>0</v>
-      </c>
-      <c r="E10" s="23">
-        <v>0</v>
-      </c>
-      <c r="F10" s="23">
-        <v>0</v>
-      </c>
-      <c r="G10" s="23">
-        <v>0</v>
-      </c>
-      <c r="H10" s="23">
-        <v>0</v>
-      </c>
-      <c r="I10" s="23">
-        <v>0</v>
-      </c>
-      <c r="J10" s="23">
-        <v>0</v>
-      </c>
-      <c r="K10" s="23">
+      <c r="B10" s="51"/>
+      <c r="C10" s="21">
+        <v>0</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0</v>
+      </c>
+      <c r="F10" s="21">
+        <v>0</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0</v>
+      </c>
+      <c r="J10" s="21">
+        <v>0</v>
+      </c>
+      <c r="K10" s="21">
         <f>SUM(C10:J10)</f>
         <v>0</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="21">
         <f>K10/A$3</f>
         <v>0</v>
       </c>
@@ -7800,39 +7807,39 @@
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="23">
-        <v>0</v>
-      </c>
-      <c r="D11" s="23">
-        <v>0</v>
-      </c>
-      <c r="E11" s="23">
-        <v>0</v>
-      </c>
-      <c r="F11" s="23">
-        <v>0</v>
-      </c>
-      <c r="G11" s="23">
-        <v>0</v>
-      </c>
-      <c r="H11" s="23">
-        <v>0</v>
-      </c>
-      <c r="I11" s="23">
-        <v>0</v>
-      </c>
-      <c r="J11" s="23">
-        <v>0</v>
-      </c>
-      <c r="K11" s="23">
+      <c r="B11" s="54"/>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
+      <c r="E11" s="21">
+        <v>0</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21">
+        <v>0</v>
+      </c>
+      <c r="J11" s="21">
+        <v>0</v>
+      </c>
+      <c r="K11" s="21">
         <f>SUM(C11:J11)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="23">
+      <c r="L11" s="21">
         <f>K11/A$3</f>
         <v>0</v>
       </c>
@@ -7845,39 +7852,39 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="23">
-        <v>0</v>
-      </c>
-      <c r="D12" s="23">
+      <c r="B12" s="49"/>
+      <c r="C12" s="21">
+        <v>0</v>
+      </c>
+      <c r="D12" s="21">
         <v>3.3</v>
       </c>
-      <c r="E12" s="23">
-        <v>0</v>
-      </c>
-      <c r="F12" s="23">
-        <v>0</v>
-      </c>
-      <c r="G12" s="23">
+      <c r="E12" s="21">
+        <v>0</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0</v>
+      </c>
+      <c r="G12" s="21">
         <v>3</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="21">
         <v>4.2</v>
       </c>
-      <c r="I12" s="23">
-        <v>0</v>
-      </c>
-      <c r="J12" s="23">
-        <v>0</v>
-      </c>
-      <c r="K12" s="23">
+      <c r="I12" s="21">
+        <v>0</v>
+      </c>
+      <c r="J12" s="21">
+        <v>0</v>
+      </c>
+      <c r="K12" s="21">
         <f>SUM(C12:J12)</f>
         <v>10.5</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="21">
         <f>K12/A$3</f>
         <v>1.3125</v>
       </c>
@@ -7890,39 +7897,39 @@
       <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="23">
-        <v>0</v>
-      </c>
-      <c r="D13" s="23">
-        <v>0</v>
-      </c>
-      <c r="E13" s="23">
-        <v>0</v>
-      </c>
-      <c r="F13" s="23">
-        <v>0</v>
-      </c>
-      <c r="G13" s="23">
-        <v>0</v>
-      </c>
-      <c r="H13" s="23">
-        <v>0</v>
-      </c>
-      <c r="I13" s="23">
-        <v>0</v>
-      </c>
-      <c r="J13" s="23">
-        <v>0</v>
-      </c>
-      <c r="K13" s="23">
+      <c r="B13" s="48"/>
+      <c r="C13" s="21">
+        <v>0</v>
+      </c>
+      <c r="D13" s="21">
+        <v>0</v>
+      </c>
+      <c r="E13" s="21">
+        <v>0</v>
+      </c>
+      <c r="F13" s="21">
+        <v>0</v>
+      </c>
+      <c r="G13" s="21">
+        <v>0</v>
+      </c>
+      <c r="H13" s="21">
+        <v>0</v>
+      </c>
+      <c r="I13" s="21">
+        <v>0</v>
+      </c>
+      <c r="J13" s="21">
+        <v>0</v>
+      </c>
+      <c r="K13" s="21">
         <f>SUM(C13:J13)</f>
         <v>0</v>
       </c>
-      <c r="L13" s="23">
+      <c r="L13" s="21">
         <f>K13/A$3</f>
         <v>0</v>
       </c>
@@ -7935,39 +7942,39 @@
       <c r="S13" s="7"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="23">
-        <v>0</v>
-      </c>
-      <c r="D14" s="23">
-        <v>0</v>
-      </c>
-      <c r="E14" s="23">
-        <v>0</v>
-      </c>
-      <c r="F14" s="23">
-        <v>0</v>
-      </c>
-      <c r="G14" s="23">
-        <v>0</v>
-      </c>
-      <c r="H14" s="23">
-        <v>0</v>
-      </c>
-      <c r="I14" s="23">
-        <v>0</v>
-      </c>
-      <c r="J14" s="23">
-        <v>0</v>
-      </c>
-      <c r="K14" s="23">
+      <c r="B14" s="48"/>
+      <c r="C14" s="21">
+        <v>0</v>
+      </c>
+      <c r="D14" s="21">
+        <v>0</v>
+      </c>
+      <c r="E14" s="21">
+        <v>0</v>
+      </c>
+      <c r="F14" s="21">
+        <v>0</v>
+      </c>
+      <c r="G14" s="21">
+        <v>0</v>
+      </c>
+      <c r="H14" s="21">
+        <v>0</v>
+      </c>
+      <c r="I14" s="21">
+        <v>0</v>
+      </c>
+      <c r="J14" s="21">
+        <v>0</v>
+      </c>
+      <c r="K14" s="21">
         <f>SUM(C14:J14)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="21">
         <f>K14/A$3</f>
         <v>0</v>
       </c>
@@ -7978,12 +7985,6 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A3:A4"/>
@@ -7998,6 +7999,12 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <conditionalFormatting sqref="C15:L96 K10:L14">
     <cfRule type="expression" dxfId="19" priority="12">
@@ -8074,20 +8081,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="33"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -8146,40 +8153,40 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34">
+      <c r="A3" s="42">
         <v>8</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="43" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -8191,18 +8198,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="34"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -8351,18 +8358,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -8428,10 +8435,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="43"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="13">
         <v>0</v>
       </c>
@@ -8473,10 +8480,10 @@
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="46"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="13">
         <v>0</v>
       </c>
@@ -8518,10 +8525,10 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="47"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="13">
         <v>0</v>
       </c>
@@ -8563,10 +8570,10 @@
       <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="41"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="13">
         <v>0</v>
       </c>
@@ -8608,10 +8615,10 @@
       <c r="S13" s="7"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="41"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="13">
         <v>0</v>
       </c>
@@ -8651,12 +8658,6 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A3:A4"/>
@@ -8671,6 +8672,12 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <conditionalFormatting sqref="C15:L96 K10:L14">
     <cfRule type="expression" dxfId="9" priority="10">

</xml_diff>